<commit_message>
more gam tries. got stuck changing perC to a gamma family
</commit_message>
<xml_diff>
--- a/data/Flett_dates_simplified_20250917.xlsx
+++ b/data/Flett_dates_simplified_20250917.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliapop/Desktop/SanJuansPaleo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DC39D2-5C8E-054B-8FD4-D89411828CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AC0782-79F0-CC49-BA2A-CF37393F3B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="760" windowWidth="27120" windowHeight="18880" xr2:uid="{5D4AA63D-30C8-2B4F-8211-9272A895DD37}"/>
   </bookViews>
@@ -288,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -296,11 +296,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -320,6 +335,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3229,7 +3245,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4533,15 +4549,15 @@
       <c r="A39" t="s">
         <v>51</v>
       </c>
-      <c r="B39">
-        <v>11.5</v>
+      <c r="B39" s="9">
+        <v>28.5</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>11.75</v>
+        <v>28.75</v>
       </c>
       <c r="E39">
         <v>10.75</v>
@@ -4569,15 +4585,15 @@
       <c r="A40" t="s">
         <v>52</v>
       </c>
-      <c r="B40">
-        <v>23.5</v>
-      </c>
-      <c r="C40">
-        <v>24</v>
+      <c r="B40" s="9">
+        <v>40.5</v>
+      </c>
+      <c r="C40" s="9">
+        <v>41</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>23.75</v>
+        <v>40.75</v>
       </c>
       <c r="E40">
         <v>17.75</v>

</xml_diff>